<commit_message>
completed checklist, test cases
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="63">
   <si>
     <t>Группа проверок/Модуль</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Браузер</t>
   </si>
   <si>
-    <t>Mozila</t>
-  </si>
-  <si>
     <t>Google Chrome</t>
   </si>
   <si>
@@ -61,6 +58,157 @@
   </si>
   <si>
     <t>Версия браузера</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Header-MENU</t>
+  </si>
+  <si>
+    <t>О НАС</t>
+  </si>
+  <si>
+    <t>НАШ СТЕК ТЕХНОЛОГИЙ МЕНЯЕТСЯ ОТ СИСТЕМЕ К СИСТЕМЕ</t>
+  </si>
+  <si>
+    <t>НАПРАВЛЕНИЯ</t>
+  </si>
+  <si>
+    <t>ПОЧЕМУ ВЫБИРАЮТ ИМЕННО НАС</t>
+  </si>
+  <si>
+    <t>РАСЧИТАЕМ ВАШ ПРОЕКТ И ПОДГОТОВИМ КОММЕРЧЕСКОЕ ПРЕДЛОЖЕНИЕ ЗА 3 ДНЯ</t>
+  </si>
+  <si>
+    <t>НАША КОМАНДА</t>
+  </si>
+  <si>
+    <t>КОНФЕРЕНЦИИ</t>
+  </si>
+  <si>
+    <t>ВАКАНСИИ</t>
+  </si>
+  <si>
+    <t>ХОЧУ РАБОТАТЬ В ITSPORTS</t>
+  </si>
+  <si>
+    <t>КОНТАКТЫ</t>
+  </si>
+  <si>
+    <t>FOOTER-NAV</t>
+  </si>
+  <si>
+    <t>Проверка кликабельности кнопки</t>
+  </si>
+  <si>
+    <t>проверка перевода страницы на языки (русский, английский)</t>
+  </si>
+  <si>
+    <t>Проверка перехода к разделам</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности кнопок и цифр для смены контента</t>
+  </si>
+  <si>
+    <t>Проверка смены изображений</t>
+  </si>
+  <si>
+    <t>Проверка смены окон с соответствующим описанием направления при нажатии на направление</t>
+  </si>
+  <si>
+    <t>Проверка кликабельности направлений</t>
+  </si>
+  <si>
+    <t>Проверка заполнения полей</t>
+  </si>
+  <si>
+    <t>Проверка отправки формы</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности кнопок</t>
+  </si>
+  <si>
+    <t>Проверка смены контента</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности кнопок, свертывание/развертывание описания вакансий</t>
+  </si>
+  <si>
+    <t>Проверка выставления/снятия галочки в чек-боксе</t>
+  </si>
+  <si>
+    <t>Проверка кнопки выхода/закрытия формы</t>
+  </si>
+  <si>
+    <t>Проверка кликабельности ссылки/перехода по ссылке</t>
+  </si>
+  <si>
+    <t>Проверка возвращения вверх страницы</t>
+  </si>
+  <si>
+    <t>Проверка названий языков</t>
+  </si>
+  <si>
+    <t>Проверка названий</t>
+  </si>
+  <si>
+    <t>Проверка названий, иконок</t>
+  </si>
+  <si>
+    <t>Проверка названий направлений, описания направлений</t>
+  </si>
+  <si>
+    <t>Проверка названий, описаний, картинок</t>
+  </si>
+  <si>
+    <t>Проверка названий полей</t>
+  </si>
+  <si>
+    <t>Проверка работы анимированых изображений</t>
+  </si>
+  <si>
+    <t>Проверка присудствия текста "Имени" анимированного изображения/должности</t>
+  </si>
+  <si>
+    <t>Проверка смены цвета фона</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности кнопоки "Я В ДЕЛЕ"/переход в форму для заполнения заявки</t>
+  </si>
+  <si>
+    <t>Проверка заполнения /отправки формы</t>
+  </si>
+  <si>
+    <t>Проверка работоспособности кнопоки для открытия формы "Я В ДЕЛЕ"</t>
+  </si>
+  <si>
+    <t>Проверка названий полей полей</t>
+  </si>
+  <si>
+    <t>Проверка присудствия анимированного изображения</t>
+  </si>
+  <si>
+    <t>Проверка названий разделов</t>
+  </si>
+  <si>
+    <t>Версия 111.0.1661.51 (Официальная сборка) (64-разрядная версия)</t>
+  </si>
+  <si>
+    <t>Версия:96.0.4693.80</t>
+  </si>
+  <si>
+    <t>Версия
+22.3.0.2430 (64-bit)</t>
+  </si>
+  <si>
+    <t>95.0.2 (64 бита)</t>
+  </si>
+  <si>
+    <t>Версия 111.0.5563.111 (Официальная сборка), (32 бит)</t>
+  </si>
+  <si>
+    <t>Safari</t>
   </si>
 </sst>
 </file>
@@ -133,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -193,11 +341,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,6 +391,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,17 +429,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,312 +733,1126 @@
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="4" width="19.21875" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="8" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="19">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="D4:I4"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B1:B5"/>
     <mergeCell ref="C1:C5"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>